<commit_message>
skill_info table / icon_atlas table
</commit_message>
<xml_diff>
--- a/로스트아크/데이터테이블/Effect_Table(수정필요-설명).xlsx
+++ b/로스트아크/데이터테이블/Effect_Table(수정필요-설명).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sky20\Desktop\진선\GameDesign\로스트아크\데이터테이블\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469B8F05-C1F9-4849-A652-1AE0CEB5EAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87EEE239-9911-4A55-AF51-A0A7FCE286B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8E3DD992-F5CA-43CA-A90A-D3D2390C4793}"/>
   </bookViews>
@@ -42,317 +42,6 @@
     <author>홍진선</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{153F9C88-79CE-4E78-9C99-B1DEE37657A0}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">ID </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>넘버링</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>규칙</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-1000 ~ 1999 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">피해형
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">2000 ~ 2999 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>능력치</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">증가
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">3000 ~ 3999 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>능력치</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">감소
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">4000 ~ 4999 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>특수기능</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> - </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">버프
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">5000 ~ 5999 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>특수기능</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> - </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">디버프
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">6000 ~ 6999 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>시너지</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">효과
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">7000 ~ 7999 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>모드</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>변경</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="C1" authorId="0" shapeId="0" xr:uid="{D8270824-394D-485A-97F5-DB008A8CB5CF}">
       <text>
         <r>
@@ -360,413 +49,26 @@
             <b/>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="돋움"/>
+            <rFont val="맑은 고딕"/>
             <family val="3"/>
             <charset val="129"/>
+            <scheme val="minor"/>
           </rPr>
-          <t>효과</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>적용</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>대상</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (enum)</t>
+          <t>효과 적용 대상</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
-SELF : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">자신
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">FOE : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">적
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">PARTY : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>파티원</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>자신</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>포함</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">) </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{44BBFA25-2682-45ED-9FFB-9541BA4459D4}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>효과</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>타입</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (enum)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-DAMAGE : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">피해
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">ABILLTY : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>능력치</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">변경
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">BUFF : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>특수기능</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">버프
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">DEBUFF : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>특수기능</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>디버프</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 
-SYNERGY : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">시너지
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">MODE : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>모드</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>변경</t>
+0 : 자신
+1 : 적
+2 : 파티원(자신 포함) </t>
         </r>
       </text>
     </comment>
@@ -775,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
   <si>
     <t>comment</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -801,10 +103,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>target</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -818,10 +116,6 @@
   </si>
   <si>
     <t>PK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>enum</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1557,10 +851,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FOE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>디버프 - 화상</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1624,14 +914,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SELF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PARTY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>시너지 - 공격력 증가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1705,10 +987,6 @@
   </si>
   <si>
     <t>No.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Affect Table의 ID 넘버링</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1739,23 +1017,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">스킬 효과 ID </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>('Affect Table의 ID 넘버링' 참고)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <rPr>
         <b/>
         <sz val="10"/>
@@ -1765,7 +1026,7 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">효과 적용 대상 </t>
+      <t xml:space="preserve">비율 연산이 필요한 지 확인 (효과 값의 적용 유형) </t>
     </r>
     <r>
       <rPr>
@@ -1789,18 +1050,18 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>SELF</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: 자신 // </t>
+      <t>0(FALSE)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 고정 수치 증감 // </t>
     </r>
     <r>
       <rPr>
@@ -1812,67 +1073,83 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>FOE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: 적 // </t>
-    </r>
+      <t>1(TRUE)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 비율 연산 후 적용  </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PARTY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: 파티원(자신 포함)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">효과 아이콘 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(Icon_Atlas_Table.xlsx의 id)
+</t>
+    </r>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">효과 타입 </t>
+        <color theme="4"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 아이콘 없음</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">효과 적용 대상 </t>
     </r>
     <r>
       <rPr>
@@ -1896,18 +1173,18 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>DAMAGE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: 피해 // </t>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 자신 // </t>
     </r>
     <r>
       <rPr>
@@ -1919,267 +1196,67 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ABILITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: 능력치 변경 // </t>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 적 // </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 파티원(자신 포함)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <color rgb="FF0070C0"/>
         <rFont val="맑은 고딕"/>
         <family val="3"/>
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>BUFF</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: 특수기능-버프 // </t>
-    </r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DEBUFF</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: 특수기능-디버프</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>//</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SYNERGY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: 시너지</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>//</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>MODE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: 모드 변경</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">효과 타입 세부 분류
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(type == DAMEGE인 경우)  dot : 도트 대미지 // 
-(type == ABILITY인 경우) 능력치 명 그대로 사용  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>atk_pwr</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> : 공격력 // </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>move_spd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> : 이동 속도 // … 
-(type == BUFF 인 경우) shield: 보호막 // ...</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">비율 연산이 필요한 지 확인 (효과 값의 적용 유형) </t>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">효과 타입 </t>
     </r>
     <r>
       <rPr>
@@ -2203,18 +1280,18 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>0(FALSE)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: 고정 수치 증감 // </t>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 피해 // </t>
     </r>
     <r>
       <rPr>
@@ -2226,73 +1303,223 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>1(TRUE)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: 비율 연산 후 적용  </t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>효과 설명</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 능력치 변경 // </t>
+    </r>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>아이콘 리소스</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 특수기능-버프 // </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
-        <color theme="4"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: 아이콘 없음(UI 표시 없음)</t>
-    </r>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 특수기능-디버프</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 시너지</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 모드 변경</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">효과 설명 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Effect_String_Table.xlsx의 id)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Effect Table의 ID 넘버링</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">스킬 효과 ID </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(우측 'Effect Table의 ID 넘버링' 참고)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>value_type</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2304,7 +1531,7 @@
     <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2358,34 +1585,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="돋움"/>
-      <family val="3"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="돋움"/>
       <family val="3"/>
       <charset val="129"/>
     </font>
@@ -2516,8 +1715,34 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2560,6 +1785,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="25">
     <border>
@@ -2877,7 +2108,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2914,140 +2145,152 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3371,10 +2614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF385D5D-99E2-46DF-BA33-B40AE917BBB4}">
-  <dimension ref="B1:J82"/>
+  <dimension ref="B1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:F5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -3393,36 +2636,36 @@
   <sheetData>
     <row r="1" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:10" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C2" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
-      <c r="H2" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" s="46"/>
-      <c r="J2" s="47"/>
+      <c r="C2" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="42"/>
+      <c r="E2" s="43"/>
+      <c r="H2" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" s="45"/>
+      <c r="J2" s="46"/>
     </row>
     <row r="3" spans="2:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C3" s="19" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="G3" s="22"/>
-      <c r="H3" s="48" t="s">
-        <v>63</v>
-      </c>
-      <c r="I3" s="49"/>
-      <c r="J3" s="50"/>
+      <c r="H3" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="48"/>
+      <c r="J3" s="49"/>
     </row>
     <row r="4" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C4" s="23" t="s">
@@ -3435,16 +2678,16 @@
         <v>1</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G4" s="22"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="53"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="52"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B5" s="26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="27">
         <v>1</v>
@@ -3456,79 +2699,77 @@
         <v>4</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G5" s="22"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="53"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="52"/>
     </row>
     <row r="6" spans="2:10" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="C6" s="31">
+      <c r="C6" s="27">
         <v>2</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G6" s="22"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="53"/>
-    </row>
-    <row r="7" spans="2:10" ht="46.8" x14ac:dyDescent="0.4">
-      <c r="C7" s="31">
+      <c r="H6" s="50"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="52"/>
+    </row>
+    <row r="7" spans="2:10" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="C7" s="27">
         <v>3</v>
       </c>
       <c r="D7" s="32" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F7" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="22"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="52"/>
+    </row>
+    <row r="8" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C8" s="27">
+        <v>4</v>
+      </c>
+      <c r="D8" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="53"/>
-    </row>
-    <row r="8" spans="2:10" ht="63" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C8" s="31">
+      <c r="E8" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="34" t="s">
-        <v>68</v>
-      </c>
+      <c r="F8" s="34"/>
       <c r="G8" s="22"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="56"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="2:10" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="C9" s="31">
+      <c r="C9" s="27">
         <v>5</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="G9" s="22"/>
       <c r="H9" s="35"/>
@@ -3536,73 +2777,65 @@
       <c r="J9" s="35"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="C10" s="31">
+      <c r="B10" s="60" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="27">
         <v>6</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="36" t="s">
-        <v>70</v>
+      <c r="E10" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="58" t="s">
+        <v>63</v>
       </c>
       <c r="G10" s="22"/>
       <c r="H10" s="35"/>
       <c r="I10" s="35"/>
       <c r="J10" s="35"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="C11" s="31"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="34"/>
+    <row r="11" spans="2:10" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="B11" s="60" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="27">
+        <v>7</v>
+      </c>
+      <c r="D11" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="59" t="s">
+        <v>60</v>
+      </c>
       <c r="G11" s="22"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B12" s="36"/>
       <c r="C12" s="31"/>
       <c r="D12" s="32"/>
       <c r="E12" s="33"/>
       <c r="F12" s="34"/>
       <c r="G12" s="22"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-    </row>
-    <row r="13" spans="2:10" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="C13" s="31">
-        <v>9</v>
-      </c>
-      <c r="D13" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="G13" s="22"/>
-      <c r="H13" s="16"/>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C13" s="37"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="40"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B14" s="37"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="22"/>
       <c r="H14" s="16"/>
     </row>
-    <row r="15" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C15" s="38"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="41"/>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="H15" s="16"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.4">
       <c r="H16" s="16"/>
@@ -3614,10 +2847,10 @@
       <c r="H18" s="16"/>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.4">
-      <c r="H19" s="16"/>
+      <c r="C19" s="16"/>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.4">
-      <c r="H20" s="16"/>
+      <c r="C20" s="16"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C21" s="16"/>
@@ -3798,12 +3031,6 @@
     </row>
     <row r="80" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C80" s="16"/>
-    </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.4">
-      <c r="C81" s="16"/>
-    </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.4">
-      <c r="C82" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3822,14 +3049,14 @@
   <dimension ref="A1:Z28"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="18.3984375" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.69921875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.19921875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="6.796875" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.69921875" style="8" customWidth="1"/>
     <col min="5" max="5" width="15.69921875" style="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="1" bestFit="1" customWidth="1"/>
@@ -3851,22 +3078,22 @@
         <v>3</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -3889,25 +3116,25 @@
     </row>
     <row r="2" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A2" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="8">
         <v>1000</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>29</v>
+      <c r="C2" s="8">
+        <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
@@ -3933,25 +3160,25 @@
     </row>
     <row r="3" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A3" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="8">
         <v>1001</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>29</v>
+      <c r="C3" s="8">
+        <v>1</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
@@ -3977,25 +3204,25 @@
     </row>
     <row r="4" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A4" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" s="8">
         <v>1002</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>29</v>
+      <c r="C4" s="8">
+        <v>1</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
@@ -4020,7 +3247,6 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="C5" s="8"/>
       <c r="G5" s="9"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -4043,7 +3269,6 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="C6" s="8"/>
       <c r="G6" s="9"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -4066,7 +3291,6 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="C7" s="8"/>
       <c r="G7" s="9"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -4089,7 +3313,6 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="C8" s="8"/>
       <c r="G8" s="9"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -4112,7 +3335,6 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="C9" s="8"/>
       <c r="G9" s="9"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -4135,7 +3357,6 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="C10" s="8"/>
       <c r="G10" s="9"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -4159,25 +3380,25 @@
     </row>
     <row r="11" spans="1:26" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" s="8">
         <v>2000</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>38</v>
+      <c r="C11" s="8">
+        <v>0</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -4201,25 +3422,25 @@
     </row>
     <row r="12" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A12" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12" s="8">
         <v>2001</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>38</v>
+      <c r="C12" s="8">
+        <v>0</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -4244,7 +3465,7 @@
     <row r="14" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
-      <c r="C14" s="6"/>
+      <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -4271,25 +3492,25 @@
     </row>
     <row r="15" spans="1:26" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A15" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B15" s="8">
         <v>3000</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>29</v>
+      <c r="C15" s="8">
+        <v>1</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -4313,25 +3534,25 @@
     </row>
     <row r="16" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A16" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16" s="8">
         <v>3001</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>29</v>
+      <c r="C16" s="8">
+        <v>1</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F16" s="1">
         <v>1</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -4356,7 +3577,7 @@
     <row r="17" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
-      <c r="C17" s="6"/>
+      <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -4383,135 +3604,135 @@
     </row>
     <row r="18" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A18" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B18" s="8">
         <v>4000</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="8">
+        <v>0</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A20" s="12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B20" s="8">
         <v>5000</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="8">
+        <v>1</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="11" t="s">
         <v>29</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A21" s="12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B21" s="8">
         <v>5100</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>29</v>
+      <c r="C21" s="8">
+        <v>1</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A23" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B23" s="8">
         <v>6000</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>29</v>
+      <c r="C23" s="8">
+        <v>1</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A24" s="12" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B24" s="8">
         <v>6001</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>39</v>
+      <c r="C24" s="8">
+        <v>2</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A26" s="12" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B26" s="8">
         <v>7000</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>38</v>
+      <c r="C26" s="8">
+        <v>0</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A27" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>38</v>
+        <v>46</v>
+      </c>
+      <c r="C27" s="8">
+        <v>0</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A28" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>38</v>
+        <v>47</v>
+      </c>
+      <c r="C28" s="8">
+        <v>0</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
skill info table 1차 완 / 그냥 enum 쓰기로 결정
</commit_message>
<xml_diff>
--- a/로스트아크/데이터테이블/Effect_Table(수정필요-설명).xlsx
+++ b/로스트아크/데이터테이블/Effect_Table(수정필요-설명).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sky20\Desktop\진선\GameDesign\로스트아크\데이터테이블\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87EEE239-9911-4A55-AF51-A0A7FCE286B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B4851B-7DFE-487E-BC57-ED6F7D1017D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8E3DD992-F5CA-43CA-A90A-D3D2390C4793}"/>
   </bookViews>
@@ -37,6 +37,265 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>홍진선</author>
+  </authors>
+  <commentList>
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{B308CCCC-AFEC-442E-BFA7-5A22CE1483FD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>ID 넘버링</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+1000 ~ 1999 : 피해형
+2000 ~ 2999 : 능력치 증가
+3000 ~ 3999 : 능력치 감소
+4000 ~ 4999 : 특수기능 - 버프
+5000 ~ 5999 : 특수기능 - 디버프
+6000 ~ 6999 : 시너지 효과
+7000 ~ 7999 : 모드 변경</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{7A13DD9A-6D13-4B12-980E-AD1338953E07}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">효과 적용 대상
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">0 : 자신
+1 : 적
+2 : 파티원(자신포함)
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{14C98F2B-D03D-4B49-A421-4C8F38342542}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>효과 타입:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>10 : 일반 피해
+11 : Dot 피해</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>20 : 능력치 증가
+21 : 능력치 감소</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>30 : 특수기능 - 버프</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> (회복, 보호막 등)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>31 : 특수기능 - 디버프</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> (상태이상, 화상 등) 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>40 : 시너지</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">50 : 모드 변경 </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">(폭주, 사신화  등)
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>홍진선</author>
@@ -77,7 +336,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="78">
   <si>
     <t>comment</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -930,10 +1189,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>type_detail</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>burn</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1002,16 +1257,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1000 ~ 1999 : 피해형
-2000 ~ 2999 : 능력치 증가
-3000 ~ 3999 : 능력치 감소
-4000 ~ 4999 : 특수기능 - 버프
-5000 ~ 5999 : 특수기능 - 디버프
-6000 ~ 6999 : 시너지 효과
-7000 ~ 7999 : 모드 변경</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>기획용 (간단한 설명)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1026,7 +1271,251 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">비율 연산이 필요한 지 확인 (효과 값의 적용 유형) </t>
+      <t xml:space="preserve">효과 아이콘 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(Icon_Atlas_Table.xlsx의 id)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 아이콘 없음</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">효과 설명 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Effect_String_Table.xlsx의 id)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">스킬 효과 ID </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(우측 'Effect Table의 ID 넘버링' 참고)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>detail_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>효과 타입의 세부 분류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">효과 타입 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(메모 참고)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>효과 적용 대상</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (메모 참고)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>→</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스킬 효과 ID 넘버링 규칙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">OO/OOO -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>효과 타입</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>효과 번호</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반 피해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1번 효과</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[예시 1] </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id = 10001</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[예시 2] </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id = 31010</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>특수기능
+- 디버프</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10번 효과</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">비율 연산이 필요한 지 확인 </t>
     </r>
     <r>
       <rPr>
@@ -1050,7 +1539,7 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>0(FALSE)</t>
+      <t>FALSE</t>
     </r>
     <r>
       <rPr>
@@ -1073,7 +1562,7 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>1(TRUE)</t>
+      <t>TRUE</t>
     </r>
     <r>
       <rPr>
@@ -1084,442 +1573,8 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">: 비율 연산 후 적용  </t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">효과 아이콘 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(Icon_Atlas_Table.xlsx의 id)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="4"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: 아이콘 없음</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">효과 적용 대상 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: 자신 // </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: 적 // </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="4"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: 파티원(자신 포함)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">효과 타입 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: 피해 // </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: 능력치 변경 // </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: 특수기능-버프 // </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: 특수기능-디버프</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>//</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: 시너지</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>//</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: 모드 변경</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">효과 설명 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Effect_String_Table.xlsx의 id)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Effect Table의 ID 넘버링</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">스킬 효과 ID </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(우측 'Effect Table의 ID 넘버링' 참고)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>value_type</t>
+      <t>: 비율 연산 후 적용</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1699,14 +1754,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF0070C0"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color theme="9"/>
@@ -1740,6 +1787,12 @@
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1781,18 +1834,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFC5"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFFFFD5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -1948,19 +2001,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="0"/>
       </left>
@@ -1971,30 +2011,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -2102,13 +2118,112 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2169,22 +2284,22 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2217,7 +2332,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2232,6 +2347,21 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2241,55 +2371,136 @@
     <xf numFmtId="0" fontId="15" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2300,10 +2511,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFFD5"/>
       <color rgb="FFFFFFC5"/>
       <color rgb="FFF9FAFD"/>
       <color rgb="FFD7DFF1"/>
-      <color rgb="FFFFFFD5"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2613,11 +2824,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF385D5D-99E2-46DF-BA33-B40AE917BBB4}">
-  <dimension ref="B1:J80"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF385D5D-99E2-46DF-BA33-B40AE917BBB4}">
+  <dimension ref="B1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2627,47 +2838,52 @@
     <col min="3" max="3" width="5.69921875" style="15" customWidth="1"/>
     <col min="4" max="4" width="18.09765625" style="16" customWidth="1"/>
     <col min="5" max="5" width="11.09765625" style="16" customWidth="1"/>
-    <col min="6" max="6" width="83.09765625" style="16" customWidth="1"/>
+    <col min="6" max="6" width="63.09765625" style="49" customWidth="1"/>
     <col min="7" max="7" width="8.69921875" style="17" customWidth="1"/>
-    <col min="8" max="8" width="11.3984375" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5" style="17" customWidth="1"/>
-    <col min="10" max="16384" width="8.796875" style="17"/>
+    <col min="8" max="8" width="8.8984375" style="18" customWidth="1"/>
+    <col min="9" max="9" width="8.8984375" style="17" customWidth="1"/>
+    <col min="10" max="11" width="8.796875" style="17"/>
+    <col min="12" max="13" width="8.796875" style="16"/>
+    <col min="14" max="16384" width="8.796875" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="2:10" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C2" s="41" t="s">
+    <row r="1" spans="2:13" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:13" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C2" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
+      <c r="H2" s="76" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="77"/>
+      <c r="J2" s="78"/>
+    </row>
+    <row r="3" spans="2:13" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C3" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="43"/>
-      <c r="H2" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2" s="45"/>
-      <c r="J2" s="46"/>
-    </row>
-    <row r="3" spans="2:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C3" s="19" t="s">
+      <c r="D3" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="E3" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="F3" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="21" t="s">
-        <v>56</v>
-      </c>
       <c r="G3" s="22"/>
-      <c r="H3" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="I3" s="48"/>
-      <c r="J3" s="49"/>
-    </row>
-    <row r="4" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="H3" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+    </row>
+    <row r="4" spans="2:13" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C4" s="23" t="s">
         <v>1</v>
       </c>
@@ -2678,14 +2894,17 @@
         <v>1</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G4" s="22"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="52"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="H4" s="74"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="75"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B5" s="26" t="s">
         <v>9</v>
       </c>
@@ -2699,15 +2918,26 @@
         <v>4</v>
       </c>
       <c r="F5" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="22"/>
+      <c r="H5" s="63" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="52"/>
-    </row>
-    <row r="6" spans="2:10" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="C6" s="27">
+      <c r="L5" s="85">
+        <v>10</v>
+      </c>
+      <c r="M5" s="86" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="C6" s="52">
         <v>2</v>
       </c>
       <c r="D6" s="32" t="s">
@@ -2716,16 +2946,23 @@
       <c r="E6" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="34" t="s">
-        <v>61</v>
+      <c r="F6" s="56" t="s">
+        <v>65</v>
       </c>
       <c r="G6" s="22"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="52"/>
-    </row>
-    <row r="7" spans="2:10" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="C7" s="27">
+      <c r="H6" s="66"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="81" t="s">
+        <v>70</v>
+      </c>
+      <c r="M6" s="87" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="C7" s="52">
         <v>3</v>
       </c>
       <c r="D7" s="32" t="s">
@@ -2734,110 +2971,142 @@
       <c r="E7" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="34" t="s">
+      <c r="F7" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="22"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="84"/>
+      <c r="J7" s="84"/>
+      <c r="K7" s="84"/>
+      <c r="L7" s="84"/>
+      <c r="M7" s="89"/>
+    </row>
+    <row r="8" spans="2:13" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C8" s="52">
+        <v>4</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="52"/>
-    </row>
-    <row r="8" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C8" s="27">
-        <v>4</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="E8" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="34" t="s">
+        <v>63</v>
+      </c>
       <c r="G8" s="22"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="55"/>
-    </row>
-    <row r="9" spans="2:10" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="C9" s="27">
+      <c r="H8" s="68" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" s="69"/>
+      <c r="J8" s="69"/>
+      <c r="K8" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="L8" s="83">
+        <v>31</v>
+      </c>
+      <c r="M8" s="90" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="31.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C9" s="52">
         <v>5</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" s="33" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="22"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="91"/>
+      <c r="L9" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="M9" s="92" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B10" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B10" s="60" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="27">
+      <c r="C10" s="57">
         <v>6</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="57" t="s">
+      <c r="E10" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="58" t="s">
-        <v>63</v>
+      <c r="F10" s="43" t="s">
+        <v>58</v>
       </c>
       <c r="G10" s="22"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-    </row>
-    <row r="11" spans="2:10" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="B11" s="60" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="27">
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="79"/>
+    </row>
+    <row r="11" spans="2:13" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="B11" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="57">
         <v>7</v>
       </c>
-      <c r="D11" s="56" t="s">
+      <c r="D11" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="57" t="s">
+      <c r="E11" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="59" t="s">
-        <v>60</v>
+      <c r="F11" s="44" t="s">
+        <v>57</v>
       </c>
       <c r="G11" s="22"/>
-      <c r="H11" s="16"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B12" s="36"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="34"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B12" s="51"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="55"/>
       <c r="G12" s="22"/>
       <c r="H12" s="16"/>
     </row>
-    <row r="13" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C13" s="37"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="40"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="H14" s="16"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B13" s="36"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="16"/>
+    </row>
+    <row r="14" spans="2:13" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C14" s="37"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="40"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.4">
       <c r="H15" s="16"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.4">
       <c r="H16" s="16"/>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.4">
@@ -2847,16 +3116,19 @@
       <c r="H18" s="16"/>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.4">
-      <c r="C19" s="16"/>
+      <c r="F19" s="50"/>
+      <c r="H19" s="16"/>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C20" s="16"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C21" s="16"/>
+      <c r="F21" s="50"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C22" s="16"/>
+      <c r="F22" s="50"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C23" s="16"/>
@@ -2866,6 +3138,7 @@
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C25" s="16"/>
+      <c r="F25" s="50"/>
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C26" s="16"/>
@@ -3032,24 +3305,33 @@
     <row r="80" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C80" s="16"/>
     </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C81" s="16"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="8">
+    <mergeCell ref="H8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="H7:M7"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H3:J8"/>
+    <mergeCell ref="H3:K4"/>
+    <mergeCell ref="H5:J6"/>
+    <mergeCell ref="K5:K6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC540C7E-1D9A-4204-BA37-262FBD0C3DDD}">
-  <dimension ref="A1:Z28"/>
+  <dimension ref="A1:Y28"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.4"/>
@@ -3061,16 +3343,16 @@
     <col min="5" max="5" width="15.69921875" style="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="15.69921875" style="11" customWidth="1"/>
-    <col min="13" max="15" width="15.69921875" style="10" customWidth="1"/>
-    <col min="16" max="17" width="15.69921875" style="11" customWidth="1"/>
-    <col min="18" max="18" width="18.69921875" style="11" customWidth="1"/>
-    <col min="19" max="22" width="15.69921875" style="10" customWidth="1"/>
-    <col min="23" max="26" width="18.69921875" style="11" customWidth="1"/>
-    <col min="27" max="16384" width="8.796875" style="2"/>
+    <col min="8" max="11" width="15.69921875" style="11" customWidth="1"/>
+    <col min="12" max="14" width="15.69921875" style="10" customWidth="1"/>
+    <col min="15" max="16" width="15.69921875" style="11" customWidth="1"/>
+    <col min="17" max="17" width="18.69921875" style="11" customWidth="1"/>
+    <col min="18" max="21" width="15.69921875" style="10" customWidth="1"/>
+    <col min="22" max="25" width="18.69921875" style="11" customWidth="1"/>
+    <col min="26" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3084,10 +3366,10 @@
         <v>5</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>2</v>
@@ -3098,23 +3380,22 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
+      <c r="L1" s="6"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
+      <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
+      <c r="R1" s="6"/>
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
       <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
+      <c r="V1" s="1"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:25" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A2" s="13" t="s">
         <v>25</v>
       </c>
@@ -3128,9 +3409,9 @@
         <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="1">
+        <v>42</v>
+      </c>
+      <c r="F2" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G2" s="9" t="s">
@@ -3142,23 +3423,22 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="L2" s="6"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
+      <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
+      <c r="R2" s="6"/>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
       <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
+      <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-    </row>
-    <row r="3" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="3" spans="1:25" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A3" s="14" t="s">
         <v>24</v>
       </c>
@@ -3172,9 +3452,9 @@
         <v>26</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="1">
+        <v>41</v>
+      </c>
+      <c r="F3" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G3" s="9" t="s">
@@ -3186,23 +3466,22 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+      <c r="L3" s="6"/>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
+      <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
+      <c r="R3" s="6"/>
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
       <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
+      <c r="V3" s="1"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-    </row>
-    <row r="4" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:25" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A4" s="13" t="s">
         <v>23</v>
       </c>
@@ -3216,9 +3495,9 @@
         <v>26</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="1">
+        <v>43</v>
+      </c>
+      <c r="F4" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G4" s="9" t="s">
@@ -3230,155 +3509,148 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
+      <c r="L4" s="6"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
+      <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
+      <c r="R4" s="6"/>
       <c r="S4" s="6"/>
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
+      <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.4">
       <c r="G5" s="9"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
+      <c r="L5" s="6"/>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
+      <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
+      <c r="R5" s="6"/>
       <c r="S5" s="6"/>
       <c r="T5" s="6"/>
       <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
+      <c r="V5" s="1"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
       <c r="G6" s="9"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
+      <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
+      <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
+      <c r="R6" s="6"/>
       <c r="S6" s="6"/>
       <c r="T6" s="6"/>
       <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
+      <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.4">
       <c r="G7" s="9"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="L7" s="6"/>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
+      <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
+      <c r="R7" s="6"/>
       <c r="S7" s="6"/>
       <c r="T7" s="6"/>
       <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
+      <c r="V7" s="1"/>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.4">
       <c r="G8" s="9"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
+      <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
+      <c r="R8" s="6"/>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
       <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
+      <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.4">
       <c r="G9" s="9"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+      <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
+      <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
+      <c r="R9" s="6"/>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
       <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
+      <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.4">
       <c r="G10" s="9"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
+      <c r="L10" s="6"/>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
+      <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
+      <c r="R10" s="6"/>
       <c r="S10" s="6"/>
       <c r="T10" s="6"/>
       <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
+      <c r="V10" s="1"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-    </row>
-    <row r="11" spans="1:26" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="1:25" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
         <v>17</v>
       </c>
@@ -3394,7 +3666,7 @@
       <c r="E11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G11" s="9" t="s">
@@ -3404,23 +3676,22 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
+      <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
+      <c r="R11" s="6"/>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
       <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
+      <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-    </row>
-    <row r="12" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="12" spans="1:25" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A12" s="7" t="s">
         <v>13</v>
       </c>
@@ -3436,7 +3707,7 @@
       <c r="E12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G12" s="9" t="s">
@@ -3446,23 +3717,22 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
+      <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
+      <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
+      <c r="R12" s="6"/>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
+      <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
-    </row>
-    <row r="14" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="14" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -3474,23 +3744,22 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
+      <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
+      <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
+      <c r="R14" s="6"/>
       <c r="S14" s="6"/>
       <c r="T14" s="6"/>
       <c r="U14" s="6"/>
-      <c r="V14" s="6"/>
+      <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-    </row>
-    <row r="15" spans="1:26" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="15" spans="1:25" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
@@ -3506,7 +3775,7 @@
       <c r="E15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G15" s="9" t="s">
@@ -3516,23 +3785,22 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
+      <c r="L15" s="6"/>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
+      <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
+      <c r="R15" s="6"/>
       <c r="S15" s="6"/>
       <c r="T15" s="6"/>
       <c r="U15" s="6"/>
-      <c r="V15" s="6"/>
+      <c r="V15" s="1"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
-    </row>
-    <row r="16" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="16" spans="1:25" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A16" s="7" t="s">
         <v>15</v>
       </c>
@@ -3548,7 +3816,7 @@
       <c r="E16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G16" s="9" t="s">
@@ -3558,23 +3826,22 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
+      <c r="L16" s="6"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
+      <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
+      <c r="R16" s="6"/>
       <c r="S16" s="6"/>
       <c r="T16" s="6"/>
       <c r="U16" s="6"/>
-      <c r="V16" s="6"/>
+      <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-    </row>
-    <row r="17" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="17" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -3586,23 +3853,22 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
+      <c r="L17" s="6"/>
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
+      <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
+      <c r="R17" s="6"/>
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
       <c r="U17" s="6"/>
-      <c r="V17" s="6"/>
+      <c r="V17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
-    </row>
-    <row r="18" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="18" spans="1:25" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A18" s="12" t="s">
         <v>21</v>
       </c>
@@ -3619,7 +3885,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:25" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A20" s="12" t="s">
         <v>27</v>
       </c>
@@ -3633,13 +3899,13 @@
         <v>31</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G20" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:25" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A21" s="12" t="s">
         <v>28</v>
       </c>
@@ -3653,10 +3919,10 @@
         <v>31</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A23" s="12" t="s">
         <v>22</v>
       </c>
@@ -3673,7 +3939,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:25" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A24" s="12" t="s">
         <v>35</v>
       </c>
@@ -3690,9 +3956,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:25" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A26" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26" s="8">
         <v>7000</v>
@@ -3704,12 +3970,12 @@
         <v>33</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A27" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C27" s="8">
         <v>0</v>
@@ -3718,12 +3984,12 @@
         <v>33</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" ht="15.6" x14ac:dyDescent="0.4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A28" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" s="8">
         <v>0</v>
@@ -3732,7 +3998,7 @@
         <v>33</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>